<commit_message>
add TAN to tag
</commit_message>
<xml_diff>
--- a/templates/community/HHU CMML/20240516_study_sheet_plant_culture.xlsx
+++ b/templates/community/HHU CMML/20240516_study_sheet_plant_culture.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2EC030-9F31-4DF1-91F6-4AE92F744F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15603DB-C1FA-4A20-A81A-82B0F5FFCC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11140" yWindow="10530" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_template" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>study template for plant culture metabolomics experiments</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C14258</t>
   </si>
 </sst>
 </file>
@@ -252,13 +255,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,9 +331,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -370,7 +371,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -476,7 +477,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -618,7 +619,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -629,17 +630,17 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -647,7 +648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -655,7 +656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -663,15 +664,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -679,49 +680,44 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>60</v>
       </c>
       <c r="C13" t="s">
@@ -731,101 +727,98 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -845,9 +838,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -918,7 +911,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>

</xml_diff>